<commit_message>
I swapped 4o to 4.1mini in results
</commit_message>
<xml_diff>
--- a/LogicBenchFiles/ResultFigures.xlsx
+++ b/LogicBenchFiles/ResultFigures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stevo\Documents\GitHub\Webscraper-ECSU\Webscraper-ECSU\LogicBenchFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{30E01D98-3542-455B-9631-5A80D9B939DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA7B905-FE28-4B35-920E-748E4757A6BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{EA2F902F-2054-488F-968C-7576C8DCD120}"/>
+    <workbookView xWindow="38055" yWindow="1560" windowWidth="28800" windowHeight="15435" xr2:uid="{EA2F902F-2054-488F-968C-7576C8DCD120}"/>
   </bookViews>
   <sheets>
     <sheet name="ResultFigures" sheetId="1" r:id="rId1"/>
@@ -67,13 +67,13 @@
     <t>Recall</t>
   </si>
   <si>
-    <t>GPT-4o-mini</t>
-  </si>
-  <si>
     <t>o3-mini</t>
   </si>
   <si>
     <t>GPT-5-mini</t>
+  </si>
+  <si>
+    <t>GPT-4.1-mini</t>
   </si>
 </sst>
 </file>
@@ -2219,7 +2219,7 @@
                   <c:v>GPT-5-mini</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>GPT-4o-mini</c:v>
+                  <c:v>GPT-4.1-mini</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>o3-mini</c:v>
@@ -2231,7 +2231,7 @@
                   <c:v>GPT-5-mini</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>GPT-4o-mini</c:v>
+                  <c:v>GPT-4.1-mini</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>o3-mini</c:v>
@@ -2243,7 +2243,7 @@
                   <c:v>GPT-5-mini</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>GPT-4o-mini</c:v>
+                  <c:v>GPT-4.1-mini</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>o3-mini</c:v>
@@ -2255,7 +2255,7 @@
                   <c:v>GPT-5-mini</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>GPT-4o-mini</c:v>
+                  <c:v>GPT-4.1-mini</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>o3-mini</c:v>
@@ -2282,7 +2282,7 @@
                   <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>40</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>80</c:v>
@@ -2291,7 +2291,7 @@
                   <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>60</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>100</c:v>
@@ -2300,7 +2300,7 @@
                   <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>80</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>100</c:v>
@@ -5241,8 +5241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E8D9040-836A-42B7-BF40-CB2A0A55683C}">
   <dimension ref="A2:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X28" sqref="X28"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5323,7 +5323,7 @@
         <v>80</v>
       </c>
       <c r="J6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K6">
         <v>80</v>
@@ -5349,7 +5349,7 @@
         <v>100</v>
       </c>
       <c r="J7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K7">
         <v>20</v>
@@ -5375,7 +5375,7 @@
         <v>80</v>
       </c>
       <c r="J8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K8">
         <v>40</v>
@@ -5415,7 +5415,7 @@
         <v>85</v>
       </c>
       <c r="J12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K12">
         <v>100</v>
@@ -5441,10 +5441,10 @@
         <v>95</v>
       </c>
       <c r="J13" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K13">
-        <v>40</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -5467,7 +5467,7 @@
         <v>95</v>
       </c>
       <c r="J14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K14">
         <v>80</v>
@@ -5507,7 +5507,7 @@
         <v>90</v>
       </c>
       <c r="J18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K18">
         <v>100</v>
@@ -5533,10 +5533,10 @@
         <v>100</v>
       </c>
       <c r="J19" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K19">
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -5559,7 +5559,7 @@
         <v>100</v>
       </c>
       <c r="J20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K20">
         <v>100</v>
@@ -5599,7 +5599,7 @@
         <v>90</v>
       </c>
       <c r="J24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K24">
         <v>100</v>
@@ -5625,10 +5625,10 @@
         <v>100</v>
       </c>
       <c r="J25" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K25">
-        <v>80</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -5651,7 +5651,7 @@
         <v>100</v>
       </c>
       <c r="J26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K26">
         <v>100</v>

</xml_diff>

<commit_message>
Added in gpt-5 results
</commit_message>
<xml_diff>
--- a/LogicBenchFiles/ResultFigures.xlsx
+++ b/LogicBenchFiles/ResultFigures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stevo\Documents\GitHub\Webscraper-ECSU\Webscraper-ECSU\LogicBenchFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA7B905-FE28-4B35-920E-748E4757A6BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34889619-323A-43FD-87EF-6108622156C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38055" yWindow="1560" windowWidth="28800" windowHeight="15435" xr2:uid="{EA2F902F-2054-488F-968C-7576C8DCD120}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{EA2F902F-2054-488F-968C-7576C8DCD120}"/>
   </bookViews>
   <sheets>
     <sheet name="ResultFigures" sheetId="1" r:id="rId1"/>
@@ -70,10 +70,10 @@
     <t>o3-mini</t>
   </si>
   <si>
-    <t>GPT-5-mini</t>
+    <t>GPT-4.1-mini</t>
   </si>
   <si>
-    <t>GPT-4.1-mini</t>
+    <t>GPT-5(-mini)</t>
   </si>
 </sst>
 </file>
@@ -2216,7 +2216,7 @@
                   <c:v>Count</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>GPT-5-mini</c:v>
+                  <c:v>GPT-5(-mini)</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>GPT-4.1-mini</c:v>
@@ -2228,7 +2228,7 @@
                   <c:v>Recall</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>GPT-5-mini</c:v>
+                  <c:v>GPT-5(-mini)</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>GPT-4.1-mini</c:v>
@@ -2240,7 +2240,7 @@
                   <c:v>Modus Ponens</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>GPT-5-mini</c:v>
+                  <c:v>GPT-5(-mini)</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>GPT-4.1-mini</c:v>
@@ -2252,7 +2252,7 @@
                   <c:v>Modus Tollens</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>GPT-5-mini</c:v>
+                  <c:v>GPT-5(-mini)</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>GPT-4.1-mini</c:v>
@@ -5241,8 +5241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E8D9040-836A-42B7-BF40-CB2A0A55683C}">
   <dimension ref="A2:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5323,7 +5323,7 @@
         <v>80</v>
       </c>
       <c r="J6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K6">
         <v>80</v>
@@ -5349,7 +5349,7 @@
         <v>100</v>
       </c>
       <c r="J7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K7">
         <v>20</v>
@@ -5415,7 +5415,7 @@
         <v>85</v>
       </c>
       <c r="J12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K12">
         <v>100</v>
@@ -5441,7 +5441,7 @@
         <v>95</v>
       </c>
       <c r="J13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K13">
         <v>80</v>
@@ -5507,7 +5507,7 @@
         <v>90</v>
       </c>
       <c r="J18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K18">
         <v>100</v>
@@ -5533,7 +5533,7 @@
         <v>100</v>
       </c>
       <c r="J19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K19">
         <v>80</v>
@@ -5599,7 +5599,7 @@
         <v>90</v>
       </c>
       <c r="J24" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K24">
         <v>100</v>
@@ -5625,7 +5625,7 @@
         <v>100</v>
       </c>
       <c r="J25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K25">
         <v>60</v>

</xml_diff>